<commit_message>
Se especifico costos de las capacitaciónes
</commit_message>
<xml_diff>
--- a/Organización/Capacitacion/Plan_capacitacion.xlsx
+++ b/Organización/Capacitacion/Plan_capacitacion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Dropbox\Repositorio\Organización\Capacitacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Capacitacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogo de cursos" sheetId="7" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="161">
   <si>
     <t>PLAN DE CAPACITACIONES</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t>Felipe Lozano</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -677,7 +680,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,12 +702,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF63776D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,7 +749,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -838,8 +835,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -859,6 +854,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1584,7 +1580,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -1605,26 +1601,26 @@
     <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -1690,7 +1686,9 @@
       <c r="D12" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F12" s="17" t="s">
         <v>127</v>
       </c>
@@ -1714,7 +1712,9 @@
       <c r="D13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="36"/>
+      <c r="E13" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F13" s="17" t="s">
         <v>127</v>
       </c>
@@ -1738,7 +1738,9 @@
       <c r="D14" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="36"/>
+      <c r="E14" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F14" s="17" t="s">
         <v>127</v>
       </c>
@@ -1762,7 +1764,9 @@
       <c r="D15" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F15" s="17" t="s">
         <v>127</v>
       </c>
@@ -1786,7 +1790,9 @@
       <c r="D16" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F16" s="17" t="s">
         <v>127</v>
       </c>
@@ -1810,7 +1816,9 @@
       <c r="D17" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F17" s="17" t="s">
         <v>127</v>
       </c>
@@ -1834,7 +1842,9 @@
       <c r="D18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F18" s="17" t="s">
         <v>127</v>
       </c>
@@ -1858,7 +1868,9 @@
       <c r="D19" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F19" s="17" t="s">
         <v>127</v>
       </c>
@@ -1882,7 +1894,9 @@
       <c r="D20" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F20" s="17" t="s">
         <v>127</v>
       </c>
@@ -1906,7 +1920,9 @@
       <c r="D21" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F21" s="17" t="s">
         <v>127</v>
       </c>
@@ -1930,7 +1946,9 @@
       <c r="D22" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F22" s="17" t="s">
         <v>127</v>
       </c>
@@ -1954,7 +1972,9 @@
       <c r="D23" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F23" s="17" t="s">
         <v>127</v>
       </c>
@@ -1978,7 +1998,9 @@
       <c r="D24" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F24" s="17" t="s">
         <v>127</v>
       </c>
@@ -2002,7 +2024,9 @@
       <c r="D25" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="36"/>
+      <c r="E25" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F25" s="17" t="s">
         <v>127</v>
       </c>
@@ -2026,7 +2050,9 @@
       <c r="D26" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="36"/>
+      <c r="E26" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F26" s="17" t="s">
         <v>127</v>
       </c>
@@ -2050,7 +2076,9 @@
       <c r="D27" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="36"/>
+      <c r="E27" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F27" s="17" t="s">
         <v>127</v>
       </c>
@@ -2074,7 +2102,9 @@
       <c r="D28" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="36"/>
+      <c r="E28" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F28" s="17" t="s">
         <v>127</v>
       </c>
@@ -2098,7 +2128,9 @@
       <c r="D29" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E29" s="36"/>
+      <c r="E29" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F29" s="17" t="s">
         <v>127</v>
       </c>
@@ -2126,7 +2158,9 @@
       <c r="D30" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F30" s="17" t="s">
         <v>127</v>
       </c>
@@ -2154,7 +2188,9 @@
       <c r="D31" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="36"/>
+      <c r="E31" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F31" s="17" t="s">
         <v>127</v>
       </c>
@@ -2182,7 +2218,9 @@
       <c r="D32" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F32" s="17" t="s">
         <v>127</v>
       </c>
@@ -2210,7 +2248,9 @@
       <c r="D33" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="36"/>
+      <c r="E33" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F33" s="17" t="s">
         <v>127</v>
       </c>
@@ -2238,7 +2278,9 @@
       <c r="D34" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="36"/>
+      <c r="E34" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F34" s="17" t="s">
         <v>127</v>
       </c>
@@ -2266,7 +2308,9 @@
       <c r="D35" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="36"/>
+      <c r="E35" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F35" s="17" t="s">
         <v>127</v>
       </c>
@@ -2294,7 +2338,9 @@
       <c r="D36" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="36"/>
+      <c r="E36" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F36" s="17" t="s">
         <v>127</v>
       </c>
@@ -2322,7 +2368,9 @@
       <c r="D37" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="36"/>
+      <c r="E37" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="F37" s="17" t="s">
         <v>127</v>
       </c>
@@ -2582,36 +2630,36 @@
     </row>
     <row r="6" spans="1:52" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -3737,7 +3785,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3756,16 +3804,16 @@
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
     </row>
     <row r="10" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
@@ -3832,44 +3880,44 @@
       <c r="D16" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3906,20 +3954,20 @@
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -3962,20 +4010,20 @@
       <c r="B12" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="36" t="s">
         <v>142</v>
       </c>
       <c r="D12" s="7">
         <v>333150296</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="37" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="37"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="7"/>
       <c r="E13" s="6"/>
     </row>
@@ -4029,46 +4077,46 @@
       <c r="E20" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Se planeó capacitación en Requerimientos y Ejecucion
</commit_message>
<xml_diff>
--- a/Organización/Capacitacion/Plan_capacitacion.xlsx
+++ b/Organización/Capacitacion/Plan_capacitacion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogo de cursos" sheetId="7" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="163">
   <si>
     <t>PLAN DE CAPACITACIONES</t>
   </si>
@@ -584,6 +584,13 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Harold Vazquez
+Carlos Gonzalez                                            Luis Humberto Vargas Alvares</t>
+  </si>
+  <si>
+    <t>29/05/2015                       10/07/2015</t>
   </si>
 </sst>
 </file>
@@ -749,7 +756,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -842,6 +849,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -854,7 +862,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1580,8 +1590,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,26 +1611,26 @@
     <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -1686,7 +1696,7 @@
       <c r="D12" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F12" s="17" t="s">
@@ -1712,7 +1722,7 @@
       <c r="D13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F13" s="17" t="s">
@@ -1738,7 +1748,7 @@
       <c r="D14" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F14" s="17" t="s">
@@ -1764,7 +1774,7 @@
       <c r="D15" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F15" s="17" t="s">
@@ -1790,7 +1800,7 @@
       <c r="D16" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F16" s="17" t="s">
@@ -1816,7 +1826,7 @@
       <c r="D17" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F17" s="17" t="s">
@@ -1842,7 +1852,7 @@
       <c r="D18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F18" s="17" t="s">
@@ -1868,7 +1878,7 @@
       <c r="D19" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F19" s="17" t="s">
@@ -1894,7 +1904,7 @@
       <c r="D20" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F20" s="17" t="s">
@@ -1920,7 +1930,7 @@
       <c r="D21" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F21" s="17" t="s">
@@ -1946,7 +1956,7 @@
       <c r="D22" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F22" s="17" t="s">
@@ -1972,7 +1982,7 @@
       <c r="D23" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F23" s="17" t="s">
@@ -1998,7 +2008,7 @@
       <c r="D24" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F24" s="17" t="s">
@@ -2024,7 +2034,7 @@
       <c r="D25" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F25" s="17" t="s">
@@ -2050,7 +2060,7 @@
       <c r="D26" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F26" s="17" t="s">
@@ -2076,7 +2086,7 @@
       <c r="D27" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F27" s="17" t="s">
@@ -2102,7 +2112,7 @@
       <c r="D28" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="42" t="s">
+      <c r="E28" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F28" s="17" t="s">
@@ -2128,7 +2138,7 @@
       <c r="D29" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F29" s="17" t="s">
@@ -2158,7 +2168,7 @@
       <c r="D30" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F30" s="17" t="s">
@@ -2188,7 +2198,7 @@
       <c r="D31" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F31" s="17" t="s">
@@ -2218,7 +2228,7 @@
       <c r="D32" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F32" s="17" t="s">
@@ -2248,7 +2258,7 @@
       <c r="D33" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F33" s="17" t="s">
@@ -2278,7 +2288,7 @@
       <c r="D34" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F34" s="17" t="s">
@@ -2308,7 +2318,7 @@
       <c r="D35" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F35" s="17" t="s">
@@ -2338,7 +2348,7 @@
       <c r="D36" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F36" s="17" t="s">
@@ -2368,7 +2378,7 @@
       <c r="D37" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="38" t="s">
         <v>160</v>
       </c>
       <c r="F37" s="17" t="s">
@@ -2588,14 +2598,14 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AZ45"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
@@ -2630,36 +2640,36 @@
     </row>
     <row r="6" spans="1:52" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -3139,8 +3149,8 @@
       <c r="D22" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="33">
-        <v>42153</v>
+      <c r="E22" s="43" t="s">
+        <v>162</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>96</v>
@@ -3149,10 +3159,10 @@
         <v>127</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="J22" s="34" t="s">
         <v>99</v>
@@ -3216,8 +3226,8 @@
       <c r="D24" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="33">
-        <v>42155</v>
+      <c r="E24" s="43" t="s">
+        <v>162</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>96</v>
@@ -3226,10 +3236,10 @@
         <v>127</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="J24" s="34" t="s">
         <v>99</v>
@@ -3804,16 +3814,16 @@
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
     </row>
     <row r="10" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
@@ -3880,44 +3890,44 @@
       <c r="D16" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3934,8 +3944,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3954,20 +3964,20 @@
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -4077,46 +4087,46 @@
       <c r="E20" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>